<commit_message>
connect clients to advisors and add a few more attributes
</commit_message>
<xml_diff>
--- a/_static/global/clients.xlsx
+++ b/_static/global/clients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eytin\Dropbox\Discrimination and Advice\experiment\findisc\_static\global\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF65DCBE-E215-46E0-9133-BA61B6D19C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E705B4-B770-425F-A98C-541E67317134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>q5</t>
+  </si>
+  <si>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>education_school</t>
+  </si>
+  <si>
+    <t>education_uni</t>
+  </si>
+  <si>
+    <t>profession</t>
   </si>
 </sst>
 </file>
@@ -440,15 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -462,34 +474,46 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -502,37 +526,37 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2">
+      <c r="I2">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G5" si="0">IF(SUM(I2:M2)&lt;=20/5+15/5,1,IF(SUM(I2:M2)&lt;=20/5+15/5*2,2,IF(SUM(I2:M2)&lt;=20/5+15/5*3,3,IF(SUM(I2:M2)&lt;=20/5+15/5*4,4,IF(SUM(I2:M2)&lt;=20/5+15/5*5,5,)))))</f>
-        <v>1</v>
-      </c>
-      <c r="H2" t="str">
-        <f t="shared" ref="H2:H6" si="1">IF(G2=1,"konservativ",IF(G2=2,"risikoscheu",IF(G2=3,"risikobereit",IF(G2=4,"spekulativ",IF(G2=5,"hochspekulativ")))))</f>
+      <c r="K2">
+        <f t="shared" ref="K2:K5" si="0">IF(SUM(M2:Q2)&lt;=20/5+15/5,1,IF(SUM(M2:Q2)&lt;=20/5+15/5*2,2,IF(SUM(M2:Q2)&lt;=20/5+15/5*3,3,IF(SUM(M2:Q2)&lt;=20/5+15/5*4,4,IF(SUM(M2:Q2)&lt;=20/5+15/5*5,5,)))))</f>
+        <v>1</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L6" si="1">IF(K2=1,"konservativ",IF(K2=2,"risikoscheu",IF(K2=3,"risikobereit",IF(K2=4,"spekulativ",IF(K2=5,"hochspekulativ")))))</f>
         <v>konservativ</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
       <c r="M2">
         <v>1</v>
       </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -545,37 +569,37 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
+      <c r="I3">
         <v>35</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="G3">
+      <c r="K3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H3" t="str">
+      <c r="L3" t="str">
         <f t="shared" si="1"/>
         <v>risikoscheu</v>
       </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
       <c r="M3">
         <v>2</v>
       </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -588,37 +612,37 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4">
+      <c r="I4">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="G4">
+      <c r="K4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H4" t="str">
+      <c r="L4" t="str">
         <f t="shared" si="1"/>
         <v>spekulativ</v>
       </c>
-      <c r="I4">
+      <c r="M4">
         <v>3</v>
       </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4">
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
         <v>3</v>
       </c>
-      <c r="L4">
-        <v>4</v>
-      </c>
-      <c r="M4">
+      <c r="P4">
+        <v>4</v>
+      </c>
+      <c r="Q4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -631,37 +655,37 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5">
+      <c r="I5">
         <v>35</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J5" t="s">
         <v>19</v>
       </c>
-      <c r="G5">
+      <c r="K5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H5" t="str">
+      <c r="L5" t="str">
         <f t="shared" si="1"/>
         <v>risikobereit</v>
       </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5">
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
         <v>3</v>
       </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -674,33 +698,33 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6">
+      <c r="I6">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
+      <c r="J6" t="s">
         <v>20</v>
       </c>
-      <c r="G6">
-        <f>IF(SUM(I6:M6)&lt;=20/4+15/5,1,IF(SUM(I6:M6)&lt;=20/4+15/5*2,2,IF(SUM(I6:M6)&lt;=20/4+15/5*3,3,IF(SUM(I6:M6)&lt;=20/4+15/5*4,4,IF(SUM(I6:M6)&lt;=20/4+15/5*5,5,)))))</f>
+      <c r="K6">
+        <f>IF(SUM(M6:Q6)&lt;=20/4+15/5,1,IF(SUM(M6:Q6)&lt;=20/4+15/5*2,2,IF(SUM(M6:Q6)&lt;=20/4+15/5*3,3,IF(SUM(M6:Q6)&lt;=20/4+15/5*4,4,IF(SUM(M6:Q6)&lt;=20/4+15/5*5,5,)))))</f>
         <v>5</v>
       </c>
-      <c r="H6" t="str">
+      <c r="L6" t="str">
         <f t="shared" si="1"/>
         <v>hochspekulativ</v>
       </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-      <c r="K6">
-        <v>4</v>
-      </c>
-      <c r="L6">
-        <v>4</v>
-      </c>
       <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
advisors: evaluation layout, risk survey
</commit_message>
<xml_diff>
--- a/_static/global/clients.xlsx
+++ b/_static/global/clients.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eytin\Dropbox\Discrimination and Advice\experiment\findisc\_static\global\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E705B4-B770-425F-A98C-541E67317134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A7D733-2079-432C-A84E-854AB0FBF388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>name</t>
   </si>
@@ -132,6 +132,69 @@
   </si>
   <si>
     <t>profession</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>evangelisch</t>
+  </si>
+  <si>
+    <t>keine</t>
+  </si>
+  <si>
+    <t>katholisch</t>
+  </si>
+  <si>
+    <t>jüdisch</t>
+  </si>
+  <si>
+    <t>muslimisch</t>
+  </si>
+  <si>
+    <t>Abitur</t>
+  </si>
+  <si>
+    <t>Hauptschulabschluss</t>
+  </si>
+  <si>
+    <t>Realschulabschluss</t>
+  </si>
+  <si>
+    <t>kein Abschluss</t>
+  </si>
+  <si>
+    <t>Fachabitur</t>
+  </si>
+  <si>
+    <t>Lehrerin</t>
+  </si>
+  <si>
+    <t>Kaufmann</t>
+  </si>
+  <si>
+    <t>Ärztin</t>
+  </si>
+  <si>
+    <t>Anwalt</t>
+  </si>
+  <si>
+    <t>HandwerkerIn</t>
+  </si>
+  <si>
+    <t>mehr als 4000€</t>
+  </si>
+  <si>
+    <t>3000-3999€</t>
+  </si>
+  <si>
+    <t>2000-2999€</t>
+  </si>
+  <si>
+    <t>1000-1999€</t>
+  </si>
+  <si>
+    <t>weniger als 1000€</t>
   </si>
 </sst>
 </file>
@@ -452,15 +515,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -486,34 +549,37 @@
         <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -526,37 +592,49 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="I2">
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2">
         <v>35</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="K2">
-        <f t="shared" ref="K2:K5" si="0">IF(SUM(M2:Q2)&lt;=20/5+15/5,1,IF(SUM(M2:Q2)&lt;=20/5+15/5*2,2,IF(SUM(M2:Q2)&lt;=20/5+15/5*3,3,IF(SUM(M2:Q2)&lt;=20/5+15/5*4,4,IF(SUM(M2:Q2)&lt;=20/5+15/5*5,5,)))))</f>
-        <v>1</v>
-      </c>
-      <c r="L2" t="str">
-        <f t="shared" ref="L2:L6" si="1">IF(K2=1,"konservativ",IF(K2=2,"risikoscheu",IF(K2=3,"risikobereit",IF(K2=4,"spekulativ",IF(K2=5,"hochspekulativ")))))</f>
-        <v>konservativ</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
+      <c r="L2">
+        <f t="shared" ref="L2:L5" si="0">IF(SUM(N2:R2)&lt;=20/5+15/5,1,IF(SUM(N2:R2)&lt;=20/5+15/5*2,2,IF(SUM(N2:R2)&lt;=20/5+15/5*3,3,IF(SUM(N2:R2)&lt;=20/5+15/5*4,4,IF(SUM(N2:R2)&lt;=20/5+15/5*5,5,)))))</f>
+        <v>4</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" ref="M2:M6" si="1">IF(L2=1,"konservativ",IF(L2=2,"risikoscheu",IF(L2=3,"risikobereit",IF(L2=4,"spekulativ",IF(L2=5,"hochspekulativ")))))</f>
+        <v>spekulativ</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="R2">
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -569,37 +647,49 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="I3">
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3">
         <v>35</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>17</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L3" t="str">
+      <c r="M3" t="str">
         <f t="shared" si="1"/>
         <v>risikoscheu</v>
       </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
       <c r="N3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O3">
         <v>2</v>
       </c>
       <c r="P3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -612,37 +702,49 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="I4">
+      <c r="E4" t="s">
         <v>35</v>
       </c>
-      <c r="J4" t="s">
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
         <v>18</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L4" t="str">
+        <v>3</v>
+      </c>
+      <c r="M4" t="str">
         <f t="shared" si="1"/>
-        <v>spekulativ</v>
-      </c>
-      <c r="M4">
+        <v>risikobereit</v>
+      </c>
+      <c r="N4">
         <v>3</v>
       </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
       <c r="O4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q4">
+        <v>4</v>
+      </c>
+      <c r="R4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -655,37 +757,49 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="I5">
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5">
         <v>35</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>19</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L5" t="str">
+        <v>1</v>
+      </c>
+      <c r="M5" t="str">
         <f t="shared" si="1"/>
-        <v>risikobereit</v>
-      </c>
-      <c r="M5">
-        <v>4</v>
+        <v>konservativ</v>
       </c>
       <c r="N5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <v>2</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q5">
         <v>1</v>
       </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -698,23 +812,32 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="I6">
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6">
         <v>35</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>20</v>
       </c>
-      <c r="K6">
-        <f>IF(SUM(M6:Q6)&lt;=20/4+15/5,1,IF(SUM(M6:Q6)&lt;=20/4+15/5*2,2,IF(SUM(M6:Q6)&lt;=20/4+15/5*3,3,IF(SUM(M6:Q6)&lt;=20/4+15/5*4,4,IF(SUM(M6:Q6)&lt;=20/4+15/5*5,5,)))))</f>
+      <c r="L6">
+        <f>IF(SUM(N6:R6)&lt;=20/4+15/5,1,IF(SUM(N6:R6)&lt;=20/4+15/5*2,2,IF(SUM(N6:R6)&lt;=20/4+15/5*3,3,IF(SUM(N6:R6)&lt;=20/4+15/5*4,4,IF(SUM(N6:R6)&lt;=20/4+15/5*5,5,)))))</f>
         <v>5</v>
       </c>
-      <c r="L6" t="str">
+      <c r="M6" t="str">
         <f t="shared" si="1"/>
         <v>hochspekulativ</v>
       </c>
-      <c r="M6">
-        <v>4</v>
-      </c>
       <c r="N6">
         <v>4</v>
       </c>
@@ -725,6 +848,284 @@
         <v>4</v>
       </c>
       <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7">
+        <v>35</v>
+      </c>
+      <c r="K7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L7:L10" si="2">IF(SUM(N7:R7)&lt;=20/5+15/5,1,IF(SUM(N7:R7)&lt;=20/5+15/5*2,2,IF(SUM(N7:R7)&lt;=20/5+15/5*3,3,IF(SUM(N7:R7)&lt;=20/5+15/5*4,4,IF(SUM(N7:R7)&lt;=20/5+15/5*5,5,)))))</f>
+        <v>4</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" ref="M7:M11" si="3">IF(L7=1,"konservativ",IF(L7=2,"risikoscheu",IF(L7=3,"risikobereit",IF(L7=4,"spekulativ",IF(L7=5,"hochspekulativ")))))</f>
+        <v>spekulativ</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8">
+        <v>35</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="3"/>
+        <v>risikoscheu</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>4</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9">
+        <v>35</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="3"/>
+        <v>risikobereit</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <v>4</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10">
+        <v>35</v>
+      </c>
+      <c r="K10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="3"/>
+        <v>konservativ</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11">
+        <v>35</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11">
+        <f>IF(SUM(N11:R11)&lt;=20/4+15/5,1,IF(SUM(N11:R11)&lt;=20/4+15/5*2,2,IF(SUM(N11:R11)&lt;=20/4+15/5*3,3,IF(SUM(N11:R11)&lt;=20/4+15/5*4,4,IF(SUM(N11:R11)&lt;=20/4+15/5*5,5,)))))</f>
+        <v>5</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="3"/>
+        <v>hochspekulativ</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
+      <c r="P11">
+        <v>4</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11">
         <v>4</v>
       </c>
     </row>

</xml_diff>